<commit_message>
Update files for original (Perma-Proto) Instructable
Updated the step-by-step doc and BOMs for the Perma-Proto version. Adds info on FET version in Step 1. BOM has updated Digi-Key link with alternate parts.
</commit_message>
<xml_diff>
--- a/docs/IV_Swinger2/Perma_Proto_construction/IV_Swinger2_BOM.xlsx
+++ b/docs/IV_Swinger2/Perma_Proto_construction/IV_Swinger2_BOM.xlsx
@@ -1,19 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csatt/GitHub/IV_Swinger/docs/IV_Swinger2/Perma_Proto_construction/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF0927C-E99F-C447-A284-E0B165687FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="0" windowWidth="30640" windowHeight="19760" tabRatio="500"/>
+    <workbookView xWindow="22140" yWindow="500" windowWidth="31220" windowHeight="25680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$F$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$F$41</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>Description</t>
   </si>
@@ -153,9 +166,6 @@
     <t>Ammeter.  Digi-Key PN: 296-1892-5-ND</t>
   </si>
   <si>
-    <t>uxcell 60 Pcs 8 Pin 2.54mm Pitch DIP IC Sockets Adaptor</t>
-  </si>
-  <si>
     <t>8-pin DIP socket (optional)</t>
   </si>
   <si>
@@ -174,12 +184,6 @@
     <t>Digi-Key PN: 1528-1195-ND</t>
   </si>
   <si>
-    <t>8mm Body Long M3 Male Female Brass Pillar Standoff Spacer 100Pcs</t>
-  </si>
-  <si>
-    <t>Came with nuts - otherwise also need 10 M3 nuts</t>
-  </si>
-  <si>
     <t>22 AWG solid core hookup wire - 6 colors - 25' each</t>
   </si>
   <si>
@@ -201,33 +205,69 @@
     <t>5V 1 Channel Relay Shield Module Optocoupler For PIC AVR DSP ARM Arduino TE213</t>
   </si>
   <si>
-    <t>Sun YOBA 5 Pairs of MC4 Male/ Female Solar Panel Cable Connectors</t>
-  </si>
-  <si>
     <t>Elegoo UNO R3 Board ATmega328P ATMEGA16U2 with USB Cable Compatible With Arduino UNO R3</t>
   </si>
   <si>
-    <t>15SQ045 Schottky bypass diodes</t>
-  </si>
-  <si>
-    <t>EFF-cientt 20pcs 15amp Diode Axial Schottky Blocking Diodes for Solar Cells Panel,15SQ045 Schottky</t>
-  </si>
-  <si>
     <t xml:space="preserve">4" Male to Female jumpers (1 blue, 1 red, 1 black) </t>
   </si>
   <si>
     <t>GenBasic 80 Piece Male to Female Solderless Ribbon Dupont Jumper Wires (4 and 8 Inch) for Breadboard Prototyping</t>
+  </si>
+  <si>
+    <t>Amazon wish list:</t>
+  </si>
+  <si>
+    <t>Digi-Key cart:</t>
+  </si>
+  <si>
+    <t>Digi-Key/Mouser CSV:</t>
+  </si>
+  <si>
+    <t>http://a.co/8RzkH2P</t>
+  </si>
+  <si>
+    <t>Only purchase items with ALT_# in Customer Reference if primary has Availability = "Backorder"</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/short/q99cnzz1</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/csatt/IV_Swinger/master/docs/IV_Swinger2/Perma_Proto_construction/PermaProto_Digikey_Mouser.csv</t>
+  </si>
+  <si>
+    <t>JYFT Solar Panel Cable Connectors Male/Female IP67 30A 1000V DC (1Pair)</t>
+  </si>
+  <si>
+    <t>15SQ100 Schottky bypass diode</t>
+  </si>
+  <si>
+    <t>Reverse connection bypass diode. Connect between binding posts. Digi-Key PN: 1655-1355-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC sockets. Recommended so ICs can be replaced more easily. Digi-Key PN: 1212-1003-ND </t>
+  </si>
+  <si>
+    <t>uxcell 20pcs M3 8+6mm Female Male Thread Brass Hex Standoff Spacer Screws PCB Pillar</t>
+  </si>
+  <si>
+    <t>M3 nuts</t>
+  </si>
+  <si>
+    <t>Standoffs</t>
+  </si>
+  <si>
+    <t>Was under $50 in 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,10 +330,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="18"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -343,7 +407,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="258">
+  <cellStyleXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -602,8 +666,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -646,7 +711,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -659,6 +723,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="258" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="258" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="258" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,7 +754,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="258">
+  <cellStyles count="259">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -933,10 +1012,31 @@
     <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1261,17 +1361,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="55" style="10" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="10"/>
@@ -1304,16 +1404,16 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" ht="17">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1321,11 +1421,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="6">
-        <v>2.67</v>
+        <v>4.09</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D10" si="0">B3*C3</f>
-        <v>2.67</v>
+        <v>4.09</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>18</v>
@@ -1334,7 +1434,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="34">
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
@@ -1342,21 +1442,21 @@
         <v>1</v>
       </c>
       <c r="C4" s="6">
-        <f>7.99/5</f>
-        <v>1.5980000000000001</v>
+        <f>8.99/5</f>
+        <v>1.798</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>1.5980000000000001</v>
+        <v>1.798</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1364,11 +1464,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="6">
-        <v>2.0499999999999998</v>
+        <v>3.77</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>7.54</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>18</v>
@@ -1377,7 +1477,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30">
+    <row r="6" spans="1:6" ht="34">
       <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
@@ -1385,21 +1485,20 @@
         <v>1</v>
       </c>
       <c r="C6" s="6">
-        <f>6.99/5</f>
-        <v>1.3980000000000001</v>
+        <v>4.99</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>1.3980000000000001</v>
+        <v>4.99</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45">
+      <c r="F6" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="51">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
@@ -1420,7 +1519,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60">
+    <row r="8" spans="1:6" ht="68">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
@@ -1428,45 +1527,44 @@
         <v>1</v>
       </c>
       <c r="C8" s="6">
-        <f>(7.99/25)*3</f>
-        <v>0.95879999999999999</v>
+        <f>(4.9/5)*3</f>
+        <v>2.9400000000000004</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>0.95879999999999999</v>
+        <v>2.9400000000000004</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34">
       <c r="A9" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B9" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="6">
-        <f>8.89/20</f>
-        <v>0.44450000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>0.88900000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34">
       <c r="A10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5">
         <v>2</v>
@@ -1482,28 +1580,28 @@
         <v>18</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="1:6" ht="17">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -1511,11 +1609,11 @@
         <v>1</v>
       </c>
       <c r="C13" s="6">
-        <v>2.98</v>
+        <v>3.77</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" ref="D13:D23" si="1">B13*C13</f>
-        <v>2.98</v>
+        <v>3.77</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>18</v>
@@ -1524,7 +1622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="17">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
@@ -1532,11 +1630,11 @@
         <v>1</v>
       </c>
       <c r="C14" s="6">
-        <v>2.58</v>
+        <v>2.82</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="1"/>
-        <v>2.58</v>
+        <v>2.82</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>18</v>
@@ -1545,7 +1643,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="17">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1553,70 +1651,69 @@
         <v>1</v>
       </c>
       <c r="C15" s="6">
-        <v>2.0499999999999998</v>
+        <v>3.04</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="1"/>
-        <v>2.0499999999999998</v>
+        <v>3.04</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17">
       <c r="A16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="5">
         <v>2</v>
       </c>
-      <c r="C16" s="19">
-        <v>0.18</v>
+      <c r="C16" s="18">
+        <v>0.26</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" si="1"/>
-        <v>0.36</v>
+        <v>0.52</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="34">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="5">
         <v>2</v>
       </c>
       <c r="C17" s="6">
-        <f>7.46/60</f>
-        <v>0.12433333333333334</v>
+        <v>0.45</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="1"/>
-        <v>0.24866666666666667</v>
+        <v>0.9</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17">
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="18">
         <f>9.59/1280</f>
         <v>7.4921874999999997E-3</v>
       </c>
@@ -1631,14 +1728,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="17">
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="18">
         <f t="shared" ref="C19:C22" si="2">9.59/1280</f>
         <v>7.4921874999999997E-3</v>
       </c>
@@ -1653,14 +1750,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="17">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="18">
         <f t="shared" si="2"/>
         <v>7.4921874999999997E-3</v>
       </c>
@@ -1675,14 +1772,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="17">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="5">
         <v>3</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="18">
         <f t="shared" si="2"/>
         <v>7.4921874999999997E-3</v>
       </c>
@@ -1697,14 +1794,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="17">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="5">
         <v>2</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="18">
         <f t="shared" si="2"/>
         <v>7.4921874999999997E-3</v>
       </c>
@@ -1719,14 +1816,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="17">
       <c r="A23" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23" s="5">
         <v>2</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="18">
         <f>4.33/100</f>
         <v>4.3299999999999998E-2</v>
       </c>
@@ -1742,24 +1839,24 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-    </row>
-    <row r="26" spans="1:6" ht="30">
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" spans="1:6" ht="34">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1767,17 +1864,17 @@
         <v>1</v>
       </c>
       <c r="C26" s="6">
-        <v>10.86</v>
+        <v>14.99</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" ref="D26:D32" si="3">B26*C26</f>
-        <v>10.86</v>
+        <f t="shared" ref="D26:D33" si="3">B26*C26</f>
+        <v>14.99</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1799,7 +1896,7 @@
       </c>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="17">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -1817,39 +1914,39 @@
         <v>18</v>
       </c>
       <c r="F28" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="34">
+      <c r="A29" s="4" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30">
-      <c r="A29" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="B29" s="5">
         <v>5</v>
       </c>
-      <c r="C29" s="20">
-        <f>16.3/125</f>
-        <v>0.13040000000000002</v>
+      <c r="C29" s="19">
+        <f>21.99/125</f>
+        <v>0.17591999999999999</v>
       </c>
       <c r="D29" s="6">
         <f t="shared" si="3"/>
-        <v>0.65200000000000014</v>
+        <v>0.87959999999999994</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="51">
       <c r="A30" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B30" s="5">
         <v>3</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="19">
         <f>5.99/80</f>
         <v>7.4874999999999997E-2</v>
       </c>
@@ -1861,10 +1958,10 @@
         <v>5</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="26">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
@@ -1872,12 +1969,12 @@
         <v>10</v>
       </c>
       <c r="C31" s="6">
-        <f>3.18/50</f>
-        <v>6.3600000000000004E-2</v>
+        <f>3.89/50</f>
+        <v>7.7800000000000008E-2</v>
       </c>
       <c r="D31" s="6">
         <f t="shared" si="3"/>
-        <v>0.63600000000000001</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>5</v>
@@ -1886,117 +1983,156 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="26">
+    <row r="32" spans="1:6" ht="17">
       <c r="A32" s="4" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B32" s="5">
         <v>10</v>
       </c>
       <c r="C32" s="6">
-        <f>5.49/100</f>
-        <v>5.4900000000000004E-2</v>
+        <f>6.29/100</f>
+        <v>6.2899999999999998E-2</v>
       </c>
       <c r="D32" s="6">
         <f t="shared" si="3"/>
-        <v>0.54900000000000004</v>
+        <v>0.629</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" customHeight="1">
+      <c r="A33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="5">
+        <v>10</v>
+      </c>
+      <c r="C33" s="6">
+        <f>5.99/20</f>
+        <v>0.29949999999999999</v>
+      </c>
+      <c r="D33" s="6">
+        <f t="shared" si="3"/>
+        <v>2.9950000000000001</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="5">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="5">
         <v>1</v>
       </c>
-      <c r="C35" s="6">
-        <v>5.2</v>
-      </c>
-      <c r="D35" s="6">
-        <f>B35*C35</f>
-        <v>5.2</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="C36" s="6">
+        <v>5.99</v>
+      </c>
+      <c r="D36" s="6">
+        <f>B36*C36</f>
+        <v>5.99</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+    </row>
+    <row r="38" spans="1:6" ht="17">
+      <c r="A38" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="13">
-        <f>SUM(D$3:D36)</f>
-        <v>48.740629166666665</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="14"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="13">
+        <f>SUM(D$3:D37)</f>
+        <v>70.520762500000004</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="24">
+      <c r="A39" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>62</v>
+      </c>
       <c r="F39" s="14"/>
     </row>
-    <row r="40" spans="1:6" ht="16" customHeight="1">
-      <c r="A40" s="16"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="12"/>
+    <row r="40" spans="1:6" ht="34">
+      <c r="A40" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="16" customHeight="1">
+      <c r="A41" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>65</v>
+      </c>
       <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="17"/>
+      <c r="A42" s="12"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="12"/>
-      <c r="F43" s="14"/>
+      <c r="A43" s="16"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="12"/>
       <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="15"/>
+      <c r="A45" s="12"/>
       <c r="F45" s="14"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="12"/>
+      <c r="A46" s="15"/>
       <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6">
@@ -2004,7 +2140,7 @@
       <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="15"/>
+      <c r="A48" s="12"/>
       <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6">
@@ -2016,7 +2152,7 @@
       <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="12"/>
+      <c r="A51" s="15"/>
       <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6">
@@ -2028,22 +2164,22 @@
       <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="9"/>
+      <c r="A54" s="12"/>
       <c r="F54" s="14"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="12"/>
+      <c r="A55" s="9"/>
       <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="12"/>
       <c r="F56" s="14"/>
     </row>
-    <row r="57" spans="1:6" ht="20" customHeight="1">
+    <row r="57" spans="1:6">
       <c r="A57" s="12"/>
       <c r="F57" s="14"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" ht="20" customHeight="1">
       <c r="A58" s="12"/>
       <c r="F58" s="14"/>
     </row>
@@ -2064,15 +2200,15 @@
       <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="18"/>
+      <c r="A63" s="12"/>
       <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="15"/>
+      <c r="A64" s="17"/>
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="12"/>
+      <c r="A65" s="15"/>
       <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6">
@@ -2085,13 +2221,13 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="12"/>
+      <c r="F68" s="14"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="18"/>
-      <c r="F69" s="14"/>
+      <c r="A69" s="12"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="12"/>
+      <c r="A70" s="17"/>
       <c r="F70" s="14"/>
     </row>
     <row r="71" spans="1:6">
@@ -2119,90 +2255,104 @@
       <c r="F76" s="14"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="17"/>
+      <c r="A77" s="12"/>
       <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="17"/>
+      <c r="A78" s="16"/>
+      <c r="F78" s="14"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="17"/>
+      <c r="A79" s="16"/>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="17"/>
+      <c r="A80" s="16"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="17"/>
+      <c r="A81" s="16"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="17"/>
+      <c r="A82" s="16"/>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="17"/>
+      <c r="A83" s="16"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="17"/>
+      <c r="A84" s="16"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="17"/>
+      <c r="A85" s="16"/>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="17"/>
+      <c r="A86" s="16"/>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="17"/>
+      <c r="A87" s="16"/>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="17"/>
+      <c r="A88" s="16"/>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="17"/>
+      <c r="A89" s="16"/>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="17"/>
+      <c r="A90" s="16"/>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="17"/>
+      <c r="A91" s="16"/>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="17"/>
+      <c r="A92" s="16"/>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="17"/>
+      <c r="A93" s="16"/>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="17"/>
+      <c r="A94" s="16"/>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="17"/>
+      <c r="A95" s="16"/>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="17"/>
+      <c r="A96" s="16"/>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="17"/>
+      <c r="A97" s="16"/>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="17"/>
+      <c r="A98" s="16"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="16"/>
     </row>
   </sheetData>
-  <sortState ref="A26:F31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A26:F31">
     <sortCondition descending="1" ref="C26:C31"/>
   </sortState>
   <mergeCells count="8">
-    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A37:F37"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$D6=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B39" r:id="rId1" xr:uid="{FC7F8BCE-D984-1640-903B-104C7D49D436}"/>
+    <hyperlink ref="B40" r:id="rId2" xr:uid="{B85F1668-B6C5-9648-9000-8BDB19DE1E36}"/>
+    <hyperlink ref="B41" r:id="rId3" xr:uid="{DE23F991-E6ED-714E-A033-3407656BEDBC}"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup scale="79" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="64" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>